<commit_message>
Added New project and codes
Signed-off-by: HANDIQUE <HANDIQUE@HANDIQUE-PC>
</commit_message>
<xml_diff>
--- a/Selenium.maven.demo/TestData/TestDataSheet.xlsx
+++ b/Selenium.maven.demo/TestData/TestDataSheet.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>test4938</t>
   </si>
@@ -27,6 +28,12 @@
   </si>
   <si>
     <t>test4545</t>
+  </si>
+  <si>
+    <t>pranjal.handique@telusinternational.com</t>
+  </si>
+  <si>
+    <t>Welcome@123</t>
   </si>
 </sst>
 </file>
@@ -382,7 +389,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -425,4 +432,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>